<commit_message>
expense ratios method added. stock split ammended
</commit_message>
<xml_diff>
--- a/outputs/holdings_output.xlsx
+++ b/outputs/holdings_output.xlsx
@@ -6023,7 +6023,7 @@
         <v>3105371</v>
       </c>
       <c r="E205" t="n">
-        <v>14379951.42589629</v>
+        <v>129419562.8330666</v>
       </c>
       <c r="F205" s="2" t="n">
         <v>45382</v>
@@ -6269,7 +6269,7 @@
         <v>3105371</v>
       </c>
       <c r="E214" t="n">
-        <v>15817946.56848592</v>
+        <v>142361519.1163732</v>
       </c>
       <c r="F214" s="2" t="n">
         <v>45473</v>
@@ -6297,7 +6297,7 @@
         <v>3105371</v>
       </c>
       <c r="E215" t="n">
-        <v>14149943.1458845</v>
+        <v>127349488.3129605</v>
       </c>
       <c r="F215" s="2" t="n">
         <v>45473</v>
@@ -6325,7 +6325,7 @@
         <v>3105371</v>
       </c>
       <c r="E216" t="n">
-        <v>14760506.07297298</v>
+        <v>132844554.6567569</v>
       </c>
       <c r="F216" s="2" t="n">
         <v>45473</v>
@@ -6353,7 +6353,7 @@
         <v>3105371</v>
       </c>
       <c r="E217" t="n">
-        <v>12653662.12277619</v>
+        <v>113882959.1049857</v>
       </c>
       <c r="F217" s="2" t="n">
         <v>45473</v>
@@ -6515,7 +6515,7 @@
         <v>3105371</v>
       </c>
       <c r="E223" t="n">
-        <v>14379951.42589629</v>
+        <v>129419562.8330666</v>
       </c>
       <c r="F223" s="2" t="n">
         <v>45565</v>
@@ -6543,7 +6543,7 @@
         <v>3105371</v>
       </c>
       <c r="E224" t="n">
-        <v>14149943.1458845</v>
+        <v>127349488.3129605</v>
       </c>
       <c r="F224" s="2" t="n">
         <v>45565</v>
@@ -6571,7 +6571,7 @@
         <v>3105371</v>
       </c>
       <c r="E225" t="n">
-        <v>13418641.8845209</v>
+        <v>120767776.9606881</v>
       </c>
       <c r="F225" s="2" t="n">
         <v>45565</v>
@@ -6599,7 +6599,7 @@
         <v>3105371</v>
       </c>
       <c r="E226" t="n">
-        <v>12653662.12277619</v>
+        <v>113882959.1049857</v>
       </c>
       <c r="F226" s="2" t="n">
         <v>45565</v>
@@ -6627,7 +6627,7 @@
         <v>3105371</v>
       </c>
       <c r="E227" t="n">
-        <v>11269119.78384732</v>
+        <v>101422078.0546259</v>
       </c>
       <c r="F227" s="2" t="n">
         <v>45565</v>
@@ -6655,7 +6655,7 @@
         <v>3105371</v>
       </c>
       <c r="E228" t="n">
-        <v>10942467.25315954</v>
+        <v>98482205.27843586</v>
       </c>
       <c r="F228" s="2" t="n">
         <v>45565</v>
@@ -6683,7 +6683,7 @@
         <v>3105371</v>
       </c>
       <c r="E229" t="n">
-        <v>9444079.803866224</v>
+        <v>84996718.23479602</v>
       </c>
       <c r="F229" s="2" t="n">
         <v>45565</v>
@@ -6763,7 +6763,7 @@
         <v>3105371</v>
       </c>
       <c r="E232" t="n">
-        <v>14379951.42589629</v>
+        <v>129419562.8330666</v>
       </c>
       <c r="F232" s="2" t="n">
         <v>45657</v>
@@ -6789,7 +6789,7 @@
         <v>3105371</v>
       </c>
       <c r="E233" t="n">
-        <v>14149943.1458845</v>
+        <v>127349488.3129605</v>
       </c>
       <c r="F233" s="2" t="n">
         <v>45657</v>
@@ -6815,7 +6815,7 @@
         <v>3105371</v>
       </c>
       <c r="E234" t="n">
-        <v>13418641.8845209</v>
+        <v>120767776.9606881</v>
       </c>
       <c r="F234" s="2" t="n">
         <v>45657</v>
@@ -6841,7 +6841,7 @@
         <v>3105371</v>
       </c>
       <c r="E235" t="n">
-        <v>12653662.12277619</v>
+        <v>113882959.1049857</v>
       </c>
       <c r="F235" s="2" t="n">
         <v>45657</v>
@@ -6867,7 +6867,7 @@
         <v>3105371</v>
       </c>
       <c r="E236" t="n">
-        <v>12396031.76223206</v>
+        <v>111564285.8600885</v>
       </c>
       <c r="F236" s="2" t="n">
         <v>45657</v>
@@ -6893,7 +6893,7 @@
         <v>3105371</v>
       </c>
       <c r="E237" t="n">
-        <v>10942467.25315954</v>
+        <v>98482205.27843586</v>
       </c>
       <c r="F237" s="2" t="n">
         <v>45657</v>
@@ -6919,7 +6919,7 @@
         <v>3105371</v>
       </c>
       <c r="E238" t="n">
-        <v>9444079.803866224</v>
+        <v>84996718.23479602</v>
       </c>
       <c r="F238" s="2" t="n">
         <v>45657</v>
@@ -6945,7 +6945,7 @@
         <v>3105371</v>
       </c>
       <c r="E239" t="n">
-        <v>9424114.370608933</v>
+        <v>84817029.33548039</v>
       </c>
       <c r="F239" s="2" t="n">
         <v>45657</v>
@@ -6971,7 +6971,7 @@
         <v>3105371</v>
       </c>
       <c r="E240" t="n">
-        <v>8501792.824446181</v>
+        <v>76516135.42001562</v>
       </c>
       <c r="F240" s="2" t="n">
         <v>45657</v>
@@ -6997,7 +6997,7 @@
         <v>3105371</v>
       </c>
       <c r="E241" t="n">
-        <v>8501792.824446181</v>
+        <v>76516135.42001562</v>
       </c>
       <c r="F241" s="2" t="n">
         <v>45657</v>
@@ -12551,7 +12551,7 @@
         <v>3105371</v>
       </c>
       <c r="E445" t="n">
-        <v>74508857.33229637</v>
+        <v>670579715.9906673</v>
       </c>
       <c r="F445" s="2" t="n">
         <v>45382</v>
@@ -12797,7 +12797,7 @@
         <v>3105371</v>
       </c>
       <c r="E454" t="n">
-        <v>81959743.06552599</v>
+        <v>737637687.589734</v>
       </c>
       <c r="F454" s="2" t="n">
         <v>45473</v>
@@ -12825,7 +12825,7 @@
         <v>3105371</v>
       </c>
       <c r="E455" t="n">
-        <v>68132962.52764796</v>
+        <v>613196662.7488316</v>
       </c>
       <c r="F455" s="2" t="n">
         <v>45473</v>
@@ -12853,7 +12853,7 @@
         <v>3105371</v>
       </c>
       <c r="E456" t="n">
-        <v>67363026.78731181</v>
+        <v>606267241.0858063</v>
       </c>
       <c r="F456" s="2" t="n">
         <v>45473</v>
@@ -12881,7 +12881,7 @@
         <v>3105371</v>
       </c>
       <c r="E457" t="n">
-        <v>79472431.95445417</v>
+        <v>715251887.5900874</v>
       </c>
       <c r="F457" s="2" t="n">
         <v>45473</v>
@@ -13043,7 +13043,7 @@
         <v>3105371</v>
       </c>
       <c r="E463" t="n">
-        <v>74508857.33229637</v>
+        <v>670579715.9906673</v>
       </c>
       <c r="F463" s="2" t="n">
         <v>45565</v>
@@ -13071,7 +13071,7 @@
         <v>3105371</v>
       </c>
       <c r="E464" t="n">
-        <v>68132962.52764796</v>
+        <v>613196662.7488316</v>
       </c>
       <c r="F464" s="2" t="n">
         <v>45565</v>
@@ -13099,7 +13099,7 @@
         <v>3105371</v>
       </c>
       <c r="E465" t="n">
-        <v>67363026.78731181</v>
+        <v>606267241.0858063</v>
       </c>
       <c r="F465" s="2" t="n">
         <v>45565</v>
@@ -13127,7 +13127,7 @@
         <v>3105371</v>
       </c>
       <c r="E466" t="n">
-        <v>79472431.95445417</v>
+        <v>715251887.5900874</v>
       </c>
       <c r="F466" s="2" t="n">
         <v>45565</v>
@@ -13155,7 +13155,7 @@
         <v>3105371</v>
       </c>
       <c r="E467" t="n">
-        <v>83999492.93166523</v>
+        <v>755995436.3849871</v>
       </c>
       <c r="F467" s="2" t="n">
         <v>45565</v>
@@ -13183,7 +13183,7 @@
         <v>3105371</v>
       </c>
       <c r="E468" t="n">
-        <v>82448522.49941714</v>
+        <v>742036702.4947542</v>
       </c>
       <c r="F468" s="2" t="n">
         <v>45565</v>
@@ -13211,7 +13211,7 @@
         <v>3105371</v>
       </c>
       <c r="E469" t="n">
-        <v>84076883.98095404</v>
+        <v>756691955.8285863</v>
       </c>
       <c r="F469" s="2" t="n">
         <v>45565</v>
@@ -13291,7 +13291,7 @@
         <v>3105371</v>
       </c>
       <c r="E472" t="n">
-        <v>74508857.33229637</v>
+        <v>670579715.9906673</v>
       </c>
       <c r="F472" s="2" t="n">
         <v>45657</v>
@@ -13317,7 +13317,7 @@
         <v>3105371</v>
       </c>
       <c r="E473" t="n">
-        <v>68132962.52764796</v>
+        <v>613196662.7488316</v>
       </c>
       <c r="F473" s="2" t="n">
         <v>45657</v>
@@ -13343,7 +13343,7 @@
         <v>3105371</v>
       </c>
       <c r="E474" t="n">
-        <v>67363026.78731181</v>
+        <v>606267241.0858063</v>
       </c>
       <c r="F474" s="2" t="n">
         <v>45657</v>
@@ -13369,7 +13369,7 @@
         <v>3105371</v>
       </c>
       <c r="E475" t="n">
-        <v>87419675.1498996</v>
+        <v>786777076.3490964</v>
       </c>
       <c r="F475" s="2" t="n">
         <v>45657</v>
@@ -13395,7 +13395,7 @@
         <v>3105371</v>
       </c>
       <c r="E476" t="n">
-        <v>83999492.93166523</v>
+        <v>755995436.3849871</v>
       </c>
       <c r="F476" s="2" t="n">
         <v>45657</v>
@@ -13421,7 +13421,7 @@
         <v>3105371</v>
       </c>
       <c r="E477" t="n">
-        <v>82448522.49941714</v>
+        <v>742036702.4947542</v>
       </c>
       <c r="F477" s="2" t="n">
         <v>45657</v>
@@ -13447,7 +13447,7 @@
         <v>3105371</v>
       </c>
       <c r="E478" t="n">
-        <v>84076883.98095404</v>
+        <v>756691955.8285863</v>
       </c>
       <c r="F478" s="2" t="n">
         <v>45657</v>
@@ -13473,7 +13473,7 @@
         <v>3105371</v>
       </c>
       <c r="E479" t="n">
-        <v>90767599.00190741</v>
+        <v>816908391.0171666</v>
       </c>
       <c r="F479" s="2" t="n">
         <v>45657</v>
@@ -13499,7 +13499,7 @@
         <v>3105371</v>
       </c>
       <c r="E480" t="n">
-        <v>109417925.0155234</v>
+        <v>984761325.1397109</v>
       </c>
       <c r="F480" s="2" t="n">
         <v>45657</v>
@@ -13525,7 +13525,7 @@
         <v>3105371</v>
       </c>
       <c r="E481" t="n">
-        <v>109417925.0155234</v>
+        <v>984761325.1397109</v>
       </c>
       <c r="F481" s="2" t="n">
         <v>45657</v>
@@ -19079,7 +19079,7 @@
         <v>3105371</v>
       </c>
       <c r="E685" t="n">
-        <v>2632392.037305259</v>
+        <v>23691528.33574733</v>
       </c>
       <c r="F685" s="2" t="n">
         <v>45382</v>
@@ -19325,7 +19325,7 @@
         <v>3105371</v>
       </c>
       <c r="E694" t="n">
-        <v>2632392.037305259</v>
+        <v>23691528.33574733</v>
       </c>
       <c r="F694" s="2" t="n">
         <v>45473</v>
@@ -19353,7 +19353,7 @@
         <v>3105371</v>
       </c>
       <c r="E695" t="n">
-        <v>2371942.533072743</v>
+        <v>21347482.79765468</v>
       </c>
       <c r="F695" s="2" t="n">
         <v>45473</v>
@@ -19381,7 +19381,7 @@
         <v>3105371</v>
       </c>
       <c r="E696" t="n">
-        <v>2194489.114371221</v>
+        <v>19750402.02934099</v>
       </c>
       <c r="F696" s="2" t="n">
         <v>45473</v>
@@ -19409,7 +19409,7 @@
         <v>3105371</v>
       </c>
       <c r="E697" t="n">
-        <v>2041749.468698347</v>
+        <v>18375745.21828512</v>
       </c>
       <c r="F697" s="2" t="n">
         <v>45473</v>
@@ -19571,7 +19571,7 @@
         <v>3105371</v>
       </c>
       <c r="E703" t="n">
-        <v>2632392.037305259</v>
+        <v>23691528.33574733</v>
       </c>
       <c r="F703" s="2" t="n">
         <v>45565</v>
@@ -19599,7 +19599,7 @@
         <v>3105371</v>
       </c>
       <c r="E704" t="n">
-        <v>2371942.533072743</v>
+        <v>21347482.79765468</v>
       </c>
       <c r="F704" s="2" t="n">
         <v>45565</v>
@@ -19627,7 +19627,7 @@
         <v>3105371</v>
       </c>
       <c r="E705" t="n">
-        <v>2194489.114371221</v>
+        <v>19750402.02934099</v>
       </c>
       <c r="F705" s="2" t="n">
         <v>45565</v>
@@ -19655,7 +19655,7 @@
         <v>3105371</v>
       </c>
       <c r="E706" t="n">
-        <v>2041749.468698347</v>
+        <v>18375745.21828512</v>
       </c>
       <c r="F706" s="2" t="n">
         <v>45565</v>
@@ -19683,7 +19683,7 @@
         <v>3105371</v>
       </c>
       <c r="E707" t="n">
-        <v>1981182.382695907</v>
+        <v>17830641.44426316</v>
       </c>
       <c r="F707" s="2" t="n">
         <v>45565</v>
@@ -19711,7 +19711,7 @@
         <v>3105371</v>
       </c>
       <c r="E708" t="n">
-        <v>1621690.823009637</v>
+        <v>14595217.40708673</v>
       </c>
       <c r="F708" s="2" t="n">
         <v>45565</v>
@@ -19739,7 +19739,7 @@
         <v>3105371</v>
       </c>
       <c r="E709" t="n">
-        <v>1583784.708300194</v>
+        <v>14254062.37470174</v>
       </c>
       <c r="F709" s="2" t="n">
         <v>45565</v>
@@ -19819,7 +19819,7 @@
         <v>3105371</v>
       </c>
       <c r="E712" t="n">
-        <v>2632392.037305259</v>
+        <v>23691528.33574733</v>
       </c>
       <c r="F712" s="2" t="n">
         <v>45657</v>
@@ -19845,7 +19845,7 @@
         <v>3105371</v>
       </c>
       <c r="E713" t="n">
-        <v>2371942.533072743</v>
+        <v>21347482.79765468</v>
       </c>
       <c r="F713" s="2" t="n">
         <v>45657</v>
@@ -19871,7 +19871,7 @@
         <v>3105371</v>
       </c>
       <c r="E714" t="n">
-        <v>2194489.114371221</v>
+        <v>19750402.02934099</v>
       </c>
       <c r="F714" s="2" t="n">
         <v>45657</v>
@@ -19897,7 +19897,7 @@
         <v>3105371</v>
       </c>
       <c r="E715" t="n">
-        <v>2041749.468698347</v>
+        <v>18375745.21828512</v>
       </c>
       <c r="F715" s="2" t="n">
         <v>45657</v>
@@ -19923,7 +19923,7 @@
         <v>3105371</v>
       </c>
       <c r="E716" t="n">
-        <v>1801074.893359914</v>
+        <v>16209674.04023923</v>
       </c>
       <c r="F716" s="2" t="n">
         <v>45657</v>
@@ -19949,7 +19949,7 @@
         <v>3105371</v>
       </c>
       <c r="E717" t="n">
-        <v>1621690.823009637</v>
+        <v>14595217.40708673</v>
       </c>
       <c r="F717" s="2" t="n">
         <v>45657</v>
@@ -19975,7 +19975,7 @@
         <v>3105371</v>
       </c>
       <c r="E718" t="n">
-        <v>1583784.708300194</v>
+        <v>14254062.37470174</v>
       </c>
       <c r="F718" s="2" t="n">
         <v>45657</v>
@@ -20001,7 +20001,7 @@
         <v>3105371</v>
       </c>
       <c r="E719" t="n">
-        <v>1578282.827605341</v>
+        <v>14204545.44844807</v>
       </c>
       <c r="F719" s="2" t="n">
         <v>45657</v>
@@ -20027,7 +20027,7 @@
         <v>3105371</v>
       </c>
       <c r="E720" t="n">
-        <v>1432397.49775516</v>
+        <v>12891577.47979644</v>
       </c>
       <c r="F720" s="2" t="n">
         <v>45657</v>
@@ -20053,7 +20053,7 @@
         <v>3105371</v>
       </c>
       <c r="E721" t="n">
-        <v>1432397.49775516</v>
+        <v>12891577.47979644</v>
       </c>
       <c r="F721" s="2" t="n">
         <v>45657</v>
@@ -25607,7 +25607,7 @@
         <v>3105371</v>
       </c>
       <c r="E925" t="n">
-        <v>591241160.1500204</v>
+        <v>5321170441.350183</v>
       </c>
       <c r="F925" s="2" t="n">
         <v>45382</v>
@@ -25853,7 +25853,7 @@
         <v>3105371</v>
       </c>
       <c r="E934" t="n">
-        <v>591241160.1500204</v>
+        <v>5321170441.350183</v>
       </c>
       <c r="F934" s="2" t="n">
         <v>45473</v>
@@ -25881,7 +25881,7 @@
         <v>3105371</v>
       </c>
       <c r="E935" t="n">
-        <v>677977263.2233633</v>
+        <v>6101795369.01027</v>
       </c>
       <c r="F935" s="2" t="n">
         <v>45473</v>
@@ -25909,7 +25909,7 @@
         <v>3105371</v>
       </c>
       <c r="E936" t="n">
-        <v>793795533.5914273</v>
+        <v>7144159802.322845</v>
       </c>
       <c r="F936" s="2" t="n">
         <v>45473</v>
@@ -25937,7 +25937,7 @@
         <v>3105371</v>
       </c>
       <c r="E937" t="n">
-        <v>839414959.7458353</v>
+        <v>7554734637.712518</v>
       </c>
       <c r="F937" s="2" t="n">
         <v>45473</v>
@@ -26099,7 +26099,7 @@
         <v>3105371</v>
       </c>
       <c r="E943" t="n">
-        <v>591241160.1500204</v>
+        <v>5321170441.350183</v>
       </c>
       <c r="F943" s="2" t="n">
         <v>45565</v>
@@ -26127,7 +26127,7 @@
         <v>3105371</v>
       </c>
       <c r="E944" t="n">
-        <v>677977263.2233633</v>
+        <v>6101795369.01027</v>
       </c>
       <c r="F944" s="2" t="n">
         <v>45565</v>
@@ -26155,7 +26155,7 @@
         <v>3105371</v>
       </c>
       <c r="E945" t="n">
-        <v>873175086.95057</v>
+        <v>7858575782.55513</v>
       </c>
       <c r="F945" s="2" t="n">
         <v>45565</v>
@@ -26183,7 +26183,7 @@
         <v>3105371</v>
       </c>
       <c r="E946" t="n">
-        <v>839414959.7458353</v>
+        <v>7554734637.712518</v>
       </c>
       <c r="F946" s="2" t="n">
         <v>45565</v>
@@ -26211,7 +26211,7 @@
         <v>3105371</v>
       </c>
       <c r="E947" t="n">
-        <v>869094958.1630133</v>
+        <v>7821854623.467119</v>
       </c>
       <c r="F947" s="2" t="n">
         <v>45565</v>
@@ -26239,7 +26239,7 @@
         <v>3105371</v>
       </c>
       <c r="E948" t="n">
-        <v>868327931.5415627</v>
+        <v>7814951383.874064</v>
       </c>
       <c r="F948" s="2" t="n">
         <v>45565</v>
@@ -26267,7 +26267,7 @@
         <v>3105371</v>
       </c>
       <c r="E949" t="n">
-        <v>934984590.5806264</v>
+        <v>8414861315.225637</v>
       </c>
       <c r="F949" s="2" t="n">
         <v>45565</v>
@@ -26347,7 +26347,7 @@
         <v>3105371</v>
       </c>
       <c r="E952" t="n">
-        <v>591241160.1500204</v>
+        <v>5321170441.350183</v>
       </c>
       <c r="F952" s="2" t="n">
         <v>45657</v>
@@ -26373,7 +26373,7 @@
         <v>3105371</v>
       </c>
       <c r="E953" t="n">
-        <v>677977263.2233633</v>
+        <v>6101795369.01027</v>
       </c>
       <c r="F953" s="2" t="n">
         <v>45657</v>
@@ -26399,7 +26399,7 @@
         <v>3105371</v>
       </c>
       <c r="E954" t="n">
-        <v>793795533.5914273</v>
+        <v>7144159802.322845</v>
       </c>
       <c r="F954" s="2" t="n">
         <v>45657</v>
@@ -26425,7 +26425,7 @@
         <v>3105371</v>
       </c>
       <c r="E955" t="n">
-        <v>839414959.7458353</v>
+        <v>7554734637.712518</v>
       </c>
       <c r="F955" s="2" t="n">
         <v>45657</v>
@@ -26451,7 +26451,7 @@
         <v>3105371</v>
       </c>
       <c r="E956" t="n">
-        <v>869094958.1630133</v>
+        <v>7821854623.467119</v>
       </c>
       <c r="F956" s="2" t="n">
         <v>45657</v>
@@ -26477,7 +26477,7 @@
         <v>3105371</v>
       </c>
       <c r="E957" t="n">
-        <v>868327931.5415627</v>
+        <v>7814951383.874064</v>
       </c>
       <c r="F957" s="2" t="n">
         <v>45657</v>
@@ -26503,7 +26503,7 @@
         <v>3105371</v>
       </c>
       <c r="E958" t="n">
-        <v>934984590.5806264</v>
+        <v>8414861315.225637</v>
       </c>
       <c r="F958" s="2" t="n">
         <v>45657</v>
@@ -26529,7 +26529,7 @@
         <v>3105371</v>
       </c>
       <c r="E959" t="n">
-        <v>968909121.7722102</v>
+        <v>8720182095.949892</v>
       </c>
       <c r="F959" s="2" t="n">
         <v>45657</v>
@@ -26555,7 +26555,7 @@
         <v>3105371</v>
       </c>
       <c r="E960" t="n">
-        <v>1003276014.377158</v>
+        <v>9029484129.394419</v>
       </c>
       <c r="F960" s="2" t="n">
         <v>45657</v>
@@ -26581,7 +26581,7 @@
         <v>3105371</v>
       </c>
       <c r="E961" t="n">
-        <v>1003276014.377158</v>
+        <v>9029484129.394419</v>
       </c>
       <c r="F961" s="2" t="n">
         <v>45657</v>
@@ -32135,7 +32135,7 @@
         <v>3105371</v>
       </c>
       <c r="E1165" t="n">
-        <v>8488256.407603649</v>
+        <v>76394307.66843285</v>
       </c>
       <c r="F1165" s="2" t="n">
         <v>45382</v>
@@ -32381,7 +32381,7 @@
         <v>3105371</v>
       </c>
       <c r="E1174" t="n">
-        <v>8488256.407603649</v>
+        <v>76394307.66843285</v>
       </c>
       <c r="F1174" s="2" t="n">
         <v>45473</v>
@@ -32409,7 +32409,7 @@
         <v>3105371</v>
       </c>
       <c r="E1175" t="n">
-        <v>8489838.365027834</v>
+        <v>76408545.2852505</v>
       </c>
       <c r="F1175" s="2" t="n">
         <v>45473</v>
@@ -32437,7 +32437,7 @@
         <v>3105371</v>
       </c>
       <c r="E1176" t="n">
-        <v>7691595.757952346</v>
+        <v>69224361.82157111</v>
       </c>
       <c r="F1176" s="2" t="n">
         <v>45473</v>
@@ -32465,7 +32465,7 @@
         <v>3105371</v>
       </c>
       <c r="E1177" t="n">
-        <v>6837892.546239044</v>
+        <v>61541032.91615139</v>
       </c>
       <c r="F1177" s="2" t="n">
         <v>45473</v>
@@ -32627,7 +32627,7 @@
         <v>3105371</v>
       </c>
       <c r="E1183" t="n">
-        <v>8488256.407603649</v>
+        <v>76394307.66843285</v>
       </c>
       <c r="F1183" s="2" t="n">
         <v>45565</v>
@@ -32655,7 +32655,7 @@
         <v>3105371</v>
       </c>
       <c r="E1184" t="n">
-        <v>8489838.365027834</v>
+        <v>76408545.2852505</v>
       </c>
       <c r="F1184" s="2" t="n">
         <v>45565</v>
@@ -32683,7 +32683,7 @@
         <v>3105371</v>
       </c>
       <c r="E1185" t="n">
-        <v>7691595.757952346</v>
+        <v>69224361.82157111</v>
       </c>
       <c r="F1185" s="2" t="n">
         <v>45565</v>
@@ -32711,7 +32711,7 @@
         <v>3105371</v>
       </c>
       <c r="E1186" t="n">
-        <v>6837892.546239044</v>
+        <v>61541032.91615139</v>
       </c>
       <c r="F1186" s="2" t="n">
         <v>45565</v>
@@ -32739,7 +32739,7 @@
         <v>3105371</v>
       </c>
       <c r="E1187" t="n">
-        <v>6529808.084413433</v>
+        <v>58768272.75972089</v>
       </c>
       <c r="F1187" s="2" t="n">
         <v>45565</v>
@@ -32767,7 +32767,7 @@
         <v>3105371</v>
       </c>
       <c r="E1188" t="n">
-        <v>5758051.697736077</v>
+        <v>51822465.27962469</v>
       </c>
       <c r="F1188" s="2" t="n">
         <v>45565</v>
@@ -32795,7 +32795,7 @@
         <v>3105371</v>
       </c>
       <c r="E1189" t="n">
-        <v>5184559.42878642</v>
+        <v>46661034.85907778</v>
       </c>
       <c r="F1189" s="2" t="n">
         <v>45565</v>
@@ -32875,7 +32875,7 @@
         <v>3105371</v>
       </c>
       <c r="E1192" t="n">
-        <v>8488256.407603649</v>
+        <v>76394307.66843285</v>
       </c>
       <c r="F1192" s="2" t="n">
         <v>45657</v>
@@ -32901,7 +32901,7 @@
         <v>3105371</v>
       </c>
       <c r="E1193" t="n">
-        <v>8489838.365027834</v>
+        <v>76408545.2852505</v>
       </c>
       <c r="F1193" s="2" t="n">
         <v>45657</v>
@@ -32927,7 +32927,7 @@
         <v>3105371</v>
       </c>
       <c r="E1194" t="n">
-        <v>7691595.757952346</v>
+        <v>69224361.82157111</v>
       </c>
       <c r="F1194" s="2" t="n">
         <v>45657</v>
@@ -32953,7 +32953,7 @@
         <v>3105371</v>
       </c>
       <c r="E1195" t="n">
-        <v>6837892.546239044</v>
+        <v>61541032.91615139</v>
       </c>
       <c r="F1195" s="2" t="n">
         <v>45657</v>
@@ -32979,7 +32979,7 @@
         <v>3105371</v>
       </c>
       <c r="E1196" t="n">
-        <v>7182788.892854776</v>
+        <v>64645100.03569299</v>
       </c>
       <c r="F1196" s="2" t="n">
         <v>45657</v>
@@ -33005,7 +33005,7 @@
         <v>3105371</v>
       </c>
       <c r="E1197" t="n">
-        <v>5758051.697736077</v>
+        <v>51822465.27962469</v>
       </c>
       <c r="F1197" s="2" t="n">
         <v>45657</v>
@@ -33031,7 +33031,7 @@
         <v>3105371</v>
       </c>
       <c r="E1198" t="n">
-        <v>5184559.42878642</v>
+        <v>46661034.85907778</v>
       </c>
       <c r="F1198" s="2" t="n">
         <v>45657</v>
@@ -33057,7 +33057,7 @@
         <v>3105371</v>
       </c>
       <c r="E1199" t="n">
-        <v>4593189.866215447</v>
+        <v>41338708.79593902</v>
       </c>
       <c r="F1199" s="2" t="n">
         <v>45657</v>
@@ -33083,7 +33083,7 @@
         <v>3105371</v>
       </c>
       <c r="E1200" t="n">
-        <v>3955033.06091629</v>
+        <v>35595297.54824661</v>
       </c>
       <c r="F1200" s="2" t="n">
         <v>45657</v>
@@ -33109,7 +33109,7 @@
         <v>3105371</v>
       </c>
       <c r="E1201" t="n">
-        <v>3955033.06091629</v>
+        <v>35595297.54824661</v>
       </c>
       <c r="F1201" s="2" t="n">
         <v>45657</v>

</xml_diff>